<commit_message>
update Due Date xlsx
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
-  <si>
-    <t>Purchase Order #:</t>
-  </si>
-  <si>
-    <t>1019705</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+  <si>
+    <t>Order #:</t>
+  </si>
+  <si>
+    <t>1020967</t>
   </si>
   <si>
     <t>Vendor:</t>
@@ -29,7 +29,7 @@
     <t>Created :</t>
   </si>
   <si>
-    <t>2021-01-26 03:21:40</t>
+    <t>2021-01-26 06:13:44</t>
   </si>
   <si>
     <t>Contact Person:</t>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Due Date:</t>
+  </si>
+  <si>
+    <t>2021-01-31 06:13:44</t>
   </si>
   <si>
     <t>Mobile:</t>
@@ -237,7 +240,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.01171875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="69.05078125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.75390625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="43.95703125" customWidth="true" bestFit="true"/>
@@ -277,313 +280,313 @@
         <v>8</v>
       </c>
       <c r="B3" t="s" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" t="n" s="3">
-        <v>0.0</v>
+        <v>250.0</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" t="n" s="3">
-        <v>0.0</v>
+        <v>250.0</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s" s="3">
         <v>26</v>
       </c>
-      <c r="B9" t="s" s="3">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s" s="3">
-        <v>25</v>
-      </c>
       <c r="D9" t="n" s="3">
-        <v>0.0</v>
+        <v>250.0</v>
       </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D10" t="n" s="3">
-        <v>0.0</v>
+        <v>106.0</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s" s="3">
         <v>31</v>
       </c>
-      <c r="B11" t="s" s="3">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s" s="3">
-        <v>30</v>
-      </c>
       <c r="D11" t="n" s="3">
-        <v>0.0</v>
+        <v>118.0</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12">
       <c r="A12" t="s" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" t="n" s="3">
-        <v>0.0</v>
+        <v>250.0</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" t="n" s="3">
-        <v>0.0</v>
+        <v>250.0</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" t="n" s="3">
-        <v>0.0</v>
+        <v>123.0</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s" s="3">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D15" t="n" s="3">
-        <v>0.0</v>
+        <v>164.0</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D16" t="n" s="3">
-        <v>0.0</v>
+        <v>250.0</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17" t="n" s="3">
-        <v>0.0</v>
+        <v>250.0</v>
       </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D18" t="n" s="3">
-        <v>0.0</v>
+        <v>250.0</v>
       </c>
       <c r="E18" s="3"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D19" t="n" s="3">
-        <v>0.0</v>
+        <v>250.0</v>
       </c>
       <c r="E19" s="3"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D20" t="n" s="3">
-        <v>0.0</v>
+        <v>250.0</v>
       </c>
       <c r="E20" s="3"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D21" t="n" s="3">
-        <v>0.0</v>
+        <v>250.0</v>
       </c>
       <c r="E21" s="3"/>
     </row>
     <row r="22">
       <c r="A22" t="s" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D22" t="n" s="3">
-        <v>0.0</v>
+        <v>250.0</v>
       </c>
       <c r="E22" s="3"/>
     </row>
     <row r="23">
       <c r="A23" t="s" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D23" t="n" s="3">
-        <v>0.0</v>
+        <v>250.0</v>
       </c>
       <c r="E23" s="3"/>
     </row>
     <row r="24">
       <c r="A24" t="s" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D24" t="n" s="3">
-        <v>0.0</v>
+        <v>250.0</v>
       </c>
       <c r="E24" s="3"/>
     </row>

</xml_diff>